<commit_message>
write groups to excel
</commit_message>
<xml_diff>
--- a/input files/player_list.xlsx
+++ b/input files/player_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Programming Projects\Python\Ranking_and_Draw\input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1234E0A1-5552-4B7D-A2A2-39D401F1897D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DE7F98-599D-4B08-8603-B9A70F62FB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u11b" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="u21m" sheetId="10" r:id="rId9"/>
     <sheet name="u21w" sheetId="11" r:id="rId10"/>
     <sheet name="mens singles" sheetId="1" r:id="rId11"/>
+    <sheet name="womens singles" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,118 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+  <si>
+    <t>Christopher Doran</t>
+  </si>
+  <si>
+    <t>Poon Yat</t>
+  </si>
+  <si>
+    <t>Adam Jepson</t>
+  </si>
+  <si>
+    <t>Shohei Nishi</t>
+  </si>
+  <si>
+    <t>Poww Poonyrapya</t>
+  </si>
+  <si>
+    <t>Howard Onweng</t>
+  </si>
+  <si>
+    <t>Djen Bakx</t>
+  </si>
+  <si>
+    <t>Luke Greenfield</t>
+  </si>
+  <si>
+    <t>Thomas Earley</t>
+  </si>
+  <si>
+    <t>Gabriel Schogger</t>
+  </si>
+  <si>
+    <t>Benjamin Dunkley</t>
+  </si>
+  <si>
+    <t>Zak Earley</t>
+  </si>
+  <si>
+    <t>David Mckenzie</t>
+  </si>
+  <si>
+    <t>James Vella Vidal</t>
+  </si>
+  <si>
+    <t>Daniel Allen</t>
+  </si>
+  <si>
+    <t>Freddie Wilke</t>
+  </si>
+  <si>
+    <t>Jakub Kurowski</t>
+  </si>
+  <si>
+    <t>Jack Sandler</t>
+  </si>
+  <si>
+    <t>Javier Goh</t>
+  </si>
+  <si>
+    <t>Max Flint</t>
+  </si>
+  <si>
+    <t>Cameron Sandhu</t>
+  </si>
+  <si>
+    <t>Scott Ching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh Yarrow </t>
+  </si>
+  <si>
+    <t>Alex Macdonell</t>
+  </si>
+  <si>
+    <t>Jaroslaw Chrzanowski</t>
+  </si>
+  <si>
+    <t>Rex Wong</t>
+  </si>
+  <si>
+    <t>Ezra Slater</t>
+  </si>
+  <si>
+    <t>Wing Tat Victor Tam</t>
+  </si>
+  <si>
+    <t>Marcus Batigin</t>
+  </si>
+  <si>
+    <t>Troy Whitham</t>
+  </si>
+  <si>
+    <t>Luca Gerrard</t>
+  </si>
+  <si>
+    <t>Helmuth Osborne</t>
+  </si>
+  <si>
+    <t>Thomas Moschidis</t>
+  </si>
+  <si>
+    <t>Chandrasekar Nittala</t>
+  </si>
+  <si>
+    <t>Deiby Sanchez</t>
+  </si>
+  <si>
+    <t>Vivian Shengwei</t>
+  </si>
+  <si>
+    <t>Joshua Bennett</t>
+  </si>
   <si>
     <t>Licence Number</t>
   </si>
@@ -46,160 +158,82 @@
     <t>County</t>
   </si>
   <si>
-    <t>Christopher Doran</t>
+    <t>Sussex</t>
+  </si>
+  <si>
+    <t>Cambridgeshire</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Derbyshire</t>
+  </si>
+  <si>
+    <t>Middlesex</t>
+  </si>
+  <si>
+    <t>Bedfordshire</t>
+  </si>
+  <si>
+    <t>Surrey</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Warwickshire</t>
+  </si>
+  <si>
+    <t>Yorkshire</t>
+  </si>
+  <si>
+    <t>South Yorkshire</t>
+  </si>
+  <si>
+    <t>Nottinghamshire</t>
   </si>
   <si>
     <t>Northamptonshire</t>
   </si>
   <si>
-    <t>Poon Yat</t>
-  </si>
-  <si>
-    <t>Nottinghamshire</t>
-  </si>
-  <si>
-    <t>Joshua Bennett</t>
-  </si>
-  <si>
-    <t>Sussex</t>
-  </si>
-  <si>
-    <t>Adam Jepson</t>
-  </si>
-  <si>
-    <t>Cambridgeshire</t>
-  </si>
-  <si>
-    <t>Shohei Nishi</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Poww Poonyrapya</t>
-  </si>
-  <si>
-    <t>Howard Onweng</t>
-  </si>
-  <si>
-    <t>Surrey</t>
-  </si>
-  <si>
-    <t>Djen Bakx</t>
-  </si>
-  <si>
     <t>Dutch</t>
   </si>
   <si>
-    <t>Luke Greenfield</t>
-  </si>
-  <si>
     <t>Leicestershire</t>
   </si>
   <si>
-    <t>Thomas Earley</t>
-  </si>
-  <si>
-    <t>Derbyshire</t>
-  </si>
-  <si>
-    <t>Gabriel Schogger</t>
-  </si>
-  <si>
-    <t>Middlesex</t>
-  </si>
-  <si>
-    <t>Benjamin Dunkley</t>
-  </si>
-  <si>
-    <t>Bedfordshire</t>
-  </si>
-  <si>
-    <t>Zak Earley</t>
-  </si>
-  <si>
-    <t>David Mckenzie</t>
-  </si>
-  <si>
-    <t>James Vella Vidal</t>
-  </si>
-  <si>
-    <t>Daniel Allen</t>
-  </si>
-  <si>
-    <t>Freddie Wilke</t>
-  </si>
-  <si>
-    <t>Kent</t>
-  </si>
-  <si>
-    <t>Jakub Kurowski</t>
-  </si>
-  <si>
-    <t>Jack Sandler</t>
-  </si>
-  <si>
-    <t>Javier Goh</t>
-  </si>
-  <si>
     <t>Buckinghamshire</t>
   </si>
   <si>
-    <t>Max Flint</t>
-  </si>
-  <si>
-    <t>Cameron Sandhu</t>
-  </si>
-  <si>
-    <t>Yorkshire</t>
-  </si>
-  <si>
-    <t>Scott Ching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josh Yarrow </t>
-  </si>
-  <si>
-    <t>Warwickshire</t>
-  </si>
-  <si>
-    <t>Alex Macdonell</t>
-  </si>
-  <si>
-    <t>Jaroslaw Chrzanowski</t>
-  </si>
-  <si>
-    <t>Rex Wong</t>
-  </si>
-  <si>
-    <t>Ezra Slater</t>
-  </si>
-  <si>
-    <t>Wing Tat Victor Tam</t>
-  </si>
-  <si>
-    <t>Marcus Batigin</t>
-  </si>
-  <si>
-    <t>Troy Whitham</t>
-  </si>
-  <si>
-    <t>South Yorkshire</t>
-  </si>
-  <si>
-    <t>Luca Gerrard</t>
-  </si>
-  <si>
-    <t>Helmuth Osborne</t>
-  </si>
-  <si>
-    <t>Thomas Moschidis</t>
-  </si>
-  <si>
-    <t>Chandrasekar Nittala</t>
-  </si>
-  <si>
-    <t>Deiby Sanchez</t>
+    <t>Lois Peake</t>
+  </si>
+  <si>
+    <t>Jasmine Wong</t>
+  </si>
+  <si>
+    <t>Scarlett Anders</t>
+  </si>
+  <si>
+    <t>Ella Pashley</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Anna Green</t>
+  </si>
+  <si>
+    <t>Anaya Patel</t>
+  </si>
+  <si>
+    <t>Berkshire</t>
+  </si>
+  <si>
+    <t>Mabel Shute</t>
+  </si>
+  <si>
+    <t>Essex</t>
   </si>
 </sst>
 </file>
@@ -531,13 +565,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -557,13 +591,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -575,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,420 +620,523 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3879</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3879</v>
+        <v>312955</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>312955</v>
+        <v>4364</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4364</v>
+        <v>1127</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1127</v>
+        <v>303928</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>303928</v>
+        <v>4904</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4904</v>
+        <v>175891</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>175891</v>
+        <v>303702</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>303702</v>
+        <v>170641</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>170641</v>
+        <v>170953</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>170953</v>
+        <v>302549</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>302549</v>
+        <v>188110</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>188110</v>
+        <v>169886</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>169886</v>
+        <v>170264</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>170264</v>
+        <v>301923</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>301923</v>
+        <v>169806</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>169806</v>
+        <v>183824</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>183824</v>
+        <v>185430</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>185430</v>
+        <v>176143</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>176143</v>
+        <v>311387</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>311387</v>
+        <v>191573</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>191573</v>
+        <v>161628</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>161628</v>
+        <v>189499</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>189499</v>
+        <v>175265</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>175265</v>
+        <v>191120</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>191120</v>
+        <v>194471</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>194471</v>
+        <v>307255</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>307255</v>
+        <v>777</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>777</v>
+        <v>315349</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>315349</v>
+        <v>161629</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>161629</v>
+        <v>306322</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>306322</v>
+        <v>199944</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>199944</v>
+        <v>2977</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2977</v>
+        <v>308973</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>308973</v>
+        <v>323795</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>323795</v>
+        <v>161691</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>161691</v>
+        <v>320803</v>
       </c>
       <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
         <v>54</v>
       </c>
-      <c r="C38" t="s">
-        <v>23</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28D3487-43C4-4AA0-8786-3EE79B33E419}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>7908</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>165375</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>182173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200336</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>156732</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>172772</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>196700</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1019,13 +1156,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1045,13 +1182,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1071,13 +1208,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1097,13 +1234,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1123,13 +1260,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1149,13 +1286,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1175,13 +1312,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1201,13 +1338,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>